<commit_message>
added Equinox API example
</commit_message>
<xml_diff>
--- a/docs/ScorecardCharacteristics.xlsx
+++ b/docs/ScorecardCharacteristics.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="272">
   <si>
     <t xml:space="preserve">EBA Index</t>
   </si>
@@ -513,6 +513,9 @@
   </si>
   <si>
     <t xml:space="preserve">Limited/weak, or local operator dependent on local authorities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.4</t>
   </si>
   <si>
     <t xml:space="preserve">Revenue Assessment</t>
@@ -1180,11 +1183,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.35"/>
@@ -2175,133 +2178,133 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>3.4</v>
+      <c r="A36" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="193.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="70.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="58.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="18" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="18" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2310,10 +2313,10 @@
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2322,10 +2325,10 @@
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F43" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2334,10 +2337,10 @@
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2346,37 +2349,37 @@
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="18" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2387,89 +2390,89 @@
         <v>14</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D47" s="15"/>
       <c r="F47" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="79.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2480,25 +2483,25 @@
         <v>14</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D51" s="15"/>
     </row>
     <row r="52" customFormat="false" ht="15.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>159</v>
@@ -2509,48 +2512,48 @@
     </row>
     <row r="53" customFormat="false" ht="135.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F53" s="16" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>98</v>
@@ -2565,10 +2568,10 @@
       </c>
       <c r="D55" s="15"/>
       <c r="E55" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="91" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2577,34 +2580,34 @@
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="58.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F57" s="16"/>
       <c r="G57" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2613,10 +2616,10 @@
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F58" s="16" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2625,10 +2628,10 @@
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2637,10 +2640,10 @@
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2649,36 +2652,36 @@
       </c>
       <c r="D61" s="15"/>
       <c r="E61" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>